<commit_message>
new csv files, new tweets
</commit_message>
<xml_diff>
--- a/Articulos/Artículos/2012-2021_LigaMX_resumen_gráficas.xlsx
+++ b/Articulos/Artículos/2012-2021_LigaMX_resumen_gráficas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Articulos\Artículos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC58C5E9-FFA6-4999-A839-549A9D37AFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0850C2-E7E8-486E-81EA-67B08656AD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1774,8 +1774,8 @@
   <dimension ref="A1:BZ37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ7" sqref="AJ7"/>
+      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>